<commit_message>
updated ui, medicaid, and subsidies
</commit_message>
<xml_diff>
--- a/data/baseline_projections.xlsx
+++ b/data/baseline_projections.xlsx
@@ -677,130 +677,130 @@
         <v>171.237</v>
       </c>
       <c r="G2" t="n">
-        <v>175.56274099593</v>
+        <v>172.825215362831</v>
       </c>
       <c r="H2" t="n">
-        <v>179.888481991861</v>
+        <v>175.416851512284</v>
       </c>
       <c r="I2" t="n">
-        <v>180.498883835544</v>
+        <v>177.199196639361</v>
       </c>
       <c r="J2" t="n">
-        <v>181.109285679227</v>
+        <v>178.999651509742</v>
       </c>
       <c r="K2" t="n">
-        <v>181.71968752291</v>
+        <v>180.818400129766</v>
       </c>
       <c r="L2" t="n">
-        <v>182.330089366593</v>
+        <v>182.655628375392</v>
       </c>
       <c r="M2" t="n">
-        <v>180.35508255879</v>
+        <v>243.397645363672</v>
       </c>
       <c r="N2" t="n">
-        <v>178.380075750986</v>
+        <v>245.827873526138</v>
       </c>
       <c r="O2" t="n">
-        <v>176.405068943183</v>
+        <v>248.28236654504</v>
       </c>
       <c r="P2" t="n">
-        <v>174.430062135379</v>
+        <v>250.761366695267</v>
       </c>
       <c r="Q2" t="n">
-        <v>175.461672281072</v>
+        <v>252.231435789332</v>
       </c>
       <c r="R2" t="n">
-        <v>176.493282426765</v>
+        <v>253.710123049624</v>
       </c>
       <c r="S2" t="n">
-        <v>177.524892572458</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>178.556502718151</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>181.209999767016</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>183.86349681588</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>186.516993864745</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>189.170490913609</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>191.812994523314</v>
+        <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>194.455498133018</v>
+        <v>0</v>
       </c>
       <c r="AA2" t="n">
-        <v>197.098001742723</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>199.740505352428</v>
+        <v>0</v>
       </c>
       <c r="AC2" t="n">
-        <v>202.769995751918</v>
+        <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>205.799486151409</v>
+        <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>208.828976550899</v>
+        <v>0</v>
       </c>
       <c r="AF2" t="n">
-        <v>211.85846695039</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="n">
-        <v>214.912515274456</v>
+        <v>0</v>
       </c>
       <c r="AH2" t="n">
-        <v>217.966563598521</v>
+        <v>0</v>
       </c>
       <c r="AI2" t="n">
-        <v>221.020611922587</v>
+        <v>0</v>
       </c>
       <c r="AJ2" t="n">
-        <v>224.074660246653</v>
+        <v>0</v>
       </c>
       <c r="AK2" t="n">
-        <v>227.230397882949</v>
+        <v>0</v>
       </c>
       <c r="AL2" t="n">
-        <v>230.386135519244</v>
+        <v>0</v>
       </c>
       <c r="AM2" t="n">
-        <v>233.54187315554</v>
+        <v>0</v>
       </c>
       <c r="AN2" t="n">
-        <v>236.697610791836</v>
+        <v>0</v>
       </c>
       <c r="AO2" t="n">
-        <v>240.027204349042</v>
+        <v>0</v>
       </c>
       <c r="AP2" t="n">
-        <v>243.356797906247</v>
+        <v>0</v>
       </c>
       <c r="AQ2" t="n">
-        <v>246.686391463453</v>
+        <v>0</v>
       </c>
       <c r="AR2" t="n">
-        <v>250.015985020658</v>
+        <v>0</v>
       </c>
       <c r="AS2" t="n">
-        <v>253.475726712435</v>
+        <v>0</v>
       </c>
       <c r="AT2" t="n">
-        <v>256.935468404212</v>
+        <v>0</v>
       </c>
       <c r="AU2" t="n">
-        <v>260.39521009599</v>
+        <v>0</v>
       </c>
       <c r="AV2" t="n">
-        <v>263.854951787767</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -823,130 +823,130 @@
         <v>145.9</v>
       </c>
       <c r="G3" t="n">
-        <v>148.620995113912</v>
+        <v>159.780785214987</v>
       </c>
       <c r="H3" t="n">
-        <v>147.797019737607</v>
+        <v>170.057946057514</v>
       </c>
       <c r="I3" t="n">
-        <v>159.242656111224</v>
+        <v>176.793058737561</v>
       </c>
       <c r="J3" t="n">
-        <v>170.909193879409</v>
+        <v>183.676060335245</v>
       </c>
       <c r="K3" t="n">
-        <v>182.800138368449</v>
+        <v>190.709714324339</v>
       </c>
       <c r="L3" t="n">
-        <v>193.820513614133</v>
+        <v>196.79829535043</v>
       </c>
       <c r="M3" t="n">
-        <v>214.404660294731</v>
+        <v>202.020669289134</v>
       </c>
       <c r="N3" t="n">
-        <v>234.020541720861</v>
+        <v>206.201363920483</v>
       </c>
       <c r="O3" t="n">
-        <v>253.778864967589</v>
+        <v>210.450353309583</v>
       </c>
       <c r="P3" t="n">
-        <v>273.526701757442</v>
+        <v>214.613968850182</v>
       </c>
       <c r="Q3" t="n">
-        <v>281.501353023059</v>
+        <v>222.279856734501</v>
       </c>
       <c r="R3" t="n">
-        <v>289.895246875818</v>
+        <v>230.338652341194</v>
       </c>
       <c r="S3" t="n">
-        <v>298.670270353253</v>
+        <v>238.752088321691</v>
       </c>
       <c r="T3" t="n">
-        <v>306.911712356143</v>
+        <v>246.605298285589</v>
       </c>
       <c r="U3" t="n">
-        <v>308.004386827056</v>
+        <v>247.052953509889</v>
       </c>
       <c r="V3" t="n">
-        <v>309.058948335501</v>
+        <v>247.29665334348</v>
       </c>
       <c r="W3" t="n">
-        <v>310.075396881479</v>
+        <v>247.333986338494</v>
       </c>
       <c r="X3" t="n">
-        <v>311.091845427458</v>
+        <v>247.200618945643</v>
       </c>
       <c r="Y3" t="n">
-        <v>312.152874549787</v>
+        <v>247.604756422399</v>
       </c>
       <c r="Z3" t="n">
-        <v>313.213903672117</v>
+        <v>247.853253102781</v>
       </c>
       <c r="AA3" t="n">
-        <v>314.313045756914</v>
+        <v>247.982091943821</v>
       </c>
       <c r="AB3" t="n">
-        <v>315.412187841712</v>
+        <v>247.951000827654</v>
       </c>
       <c r="AC3" t="n">
-        <v>314.980134697246</v>
+        <v>246.788242201678</v>
       </c>
       <c r="AD3" t="n">
-        <v>314.54808155278</v>
+        <v>245.432408562552</v>
       </c>
       <c r="AE3" t="n">
-        <v>314.154141370781</v>
+        <v>243.918748838027</v>
       </c>
       <c r="AF3" t="n">
-        <v>313.79831415125</v>
+        <v>242.244356508887</v>
       </c>
       <c r="AG3" t="n">
-        <v>313.342899676483</v>
+        <v>241.038171302294</v>
       </c>
       <c r="AH3" t="n">
-        <v>312.887485201714</v>
+        <v>239.646592519882</v>
       </c>
       <c r="AI3" t="n">
-        <v>312.470183689414</v>
+        <v>238.105116499942</v>
       </c>
       <c r="AJ3" t="n">
-        <v>312.052882177113</v>
+        <v>236.372976725091</v>
       </c>
       <c r="AK3" t="n">
-        <v>311.261323296029</v>
+        <v>234.799177029243</v>
       </c>
       <c r="AL3" t="n">
-        <v>310.469764414943</v>
+        <v>233.038045405906</v>
       </c>
       <c r="AM3" t="n">
-        <v>309.678205533858</v>
+        <v>231.086997551258</v>
       </c>
       <c r="AN3" t="n">
-        <v>308.924759615241</v>
+        <v>228.981526472646</v>
       </c>
       <c r="AO3" t="n">
-        <v>307.542519377805</v>
+        <v>226.773609543596</v>
       </c>
       <c r="AP3" t="n">
-        <v>306.198392102836</v>
+        <v>224.406376101317</v>
       </c>
       <c r="AQ3" t="n">
-        <v>304.930490752802</v>
+        <v>221.915218642343</v>
       </c>
       <c r="AR3" t="n">
-        <v>303.738815327704</v>
+        <v>219.297379214267</v>
       </c>
       <c r="AS3" t="n">
-        <v>302.095589326862</v>
+        <v>321.720903844883</v>
       </c>
       <c r="AT3" t="n">
-        <v>300.528589250955</v>
+        <v>416.839625234504</v>
       </c>
       <c r="AU3" t="n">
-        <v>299.07592806245</v>
+        <v>505.29673765003</v>
       </c>
       <c r="AV3" t="n">
-        <v>297.661379836413</v>
+        <v>587.57149317354</v>
       </c>
     </row>
     <row r="4">
@@ -1261,130 +1261,130 @@
         <v>1403.263</v>
       </c>
       <c r="G6" t="n">
-        <v>1394.63952711825</v>
+        <v>1386.21726265027</v>
       </c>
       <c r="H6" t="n">
-        <v>1386.0160542365</v>
+        <v>1368.22675839617</v>
       </c>
       <c r="I6" t="n">
-        <v>1416.24742986613</v>
+        <v>1401.99671443597</v>
       </c>
       <c r="J6" t="n">
-        <v>1446.47880549575</v>
+        <v>1435.8215732094</v>
       </c>
       <c r="K6" t="n">
-        <v>1476.71018112537</v>
+        <v>1469.70189256263</v>
       </c>
       <c r="L6" t="n">
-        <v>1506.941556755</v>
+        <v>1503.6382360099</v>
       </c>
       <c r="M6" t="n">
-        <v>1519.7601557668</v>
+        <v>1469.10158396751</v>
       </c>
       <c r="N6" t="n">
-        <v>1532.57875477859</v>
+        <v>1492.95013480382</v>
       </c>
       <c r="O6" t="n">
-        <v>1545.39735379039</v>
+        <v>1516.84856784654</v>
       </c>
       <c r="P6" t="n">
-        <v>1558.21595280219</v>
+        <v>1540.79738114956</v>
       </c>
       <c r="Q6" t="n">
-        <v>1568.7825477364</v>
+        <v>1551.2342805167</v>
       </c>
       <c r="R6" t="n">
-        <v>1579.34914267061</v>
+        <v>1561.68889658237</v>
       </c>
       <c r="S6" t="n">
-        <v>1589.91573760481</v>
+        <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>1600.48233253902</v>
+        <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>1639.9186754518</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>1679.35501836459</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>1718.79136127737</v>
+        <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>1758.22770419015</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>1787.6196955995</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>1817.01168700885</v>
+        <v>0</v>
       </c>
       <c r="AA6" t="n">
-        <v>1846.40367841819</v>
+        <v>0</v>
       </c>
       <c r="AB6" t="n">
-        <v>1875.79566982754</v>
+        <v>0</v>
       </c>
       <c r="AC6" t="n">
-        <v>1908.21487279363</v>
+        <v>0</v>
       </c>
       <c r="AD6" t="n">
-        <v>1940.63407575972</v>
+        <v>0</v>
       </c>
       <c r="AE6" t="n">
-        <v>1973.05327872581</v>
+        <v>0</v>
       </c>
       <c r="AF6" t="n">
-        <v>2005.4724816919</v>
+        <v>0</v>
       </c>
       <c r="AG6" t="n">
-        <v>2057.17598732875</v>
+        <v>0</v>
       </c>
       <c r="AH6" t="n">
-        <v>2108.87949296561</v>
+        <v>0</v>
       </c>
       <c r="AI6" t="n">
-        <v>2160.58299860246</v>
+        <v>0</v>
       </c>
       <c r="AJ6" t="n">
-        <v>2212.28650423931</v>
+        <v>0</v>
       </c>
       <c r="AK6" t="n">
-        <v>2211.53431384661</v>
+        <v>0</v>
       </c>
       <c r="AL6" t="n">
-        <v>2210.78212345391</v>
+        <v>0</v>
       </c>
       <c r="AM6" t="n">
-        <v>2210.0299330612</v>
+        <v>0</v>
       </c>
       <c r="AN6" t="n">
-        <v>2209.2777426685</v>
+        <v>0</v>
       </c>
       <c r="AO6" t="n">
-        <v>2261.64930877257</v>
+        <v>0</v>
       </c>
       <c r="AP6" t="n">
-        <v>2314.02087487663</v>
+        <v>0</v>
       </c>
       <c r="AQ6" t="n">
-        <v>2366.3924409807</v>
+        <v>0</v>
       </c>
       <c r="AR6" t="n">
-        <v>2418.76400708477</v>
+        <v>0</v>
       </c>
       <c r="AS6" t="n">
-        <v>2464.36520513099</v>
+        <v>0</v>
       </c>
       <c r="AT6" t="n">
-        <v>2509.9664031772</v>
+        <v>0</v>
       </c>
       <c r="AU6" t="n">
-        <v>2555.56760122341</v>
+        <v>0</v>
       </c>
       <c r="AV6" t="n">
-        <v>2601.16879926962</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">

</xml_diff>